<commit_message>
Created logic for farm implement.
</commit_message>
<xml_diff>
--- a/Content/Tractor_images/tractorimg3.xlsx
+++ b/Content/Tractor_images/tractorimg3.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>New Holland Tractors</t>
-  </si>
-  <si>
-    <t>4510</t>
-  </si>
-  <si>
-    <t>['4510img0-4510-1632217675.png', '4510img1-upload-1632217675-0.png', '4510img2-4510-1632217675.png']</t>
+    <t>Mahindra</t>
+  </si>
+  <si>
+    <t>Gahir-800</t>
+  </si>
+  <si>
+    <t>['Gahir-800img0-gahir-800-1649326242.png']</t>
   </si>
   <si>
     <t>Brand</t>

</xml_diff>